<commit_message>
Convert.py now running for all ontology-templates in excel-file
</commit_message>
<xml_diff>
--- a/Master_Table/Possible_Template_TF_OntoWorldMap_2023-03-28_10-52.xlsx
+++ b/Master_Table/Possible_Template_TF_OntoWorldMap_2023-03-28_10-52.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smaxbehr\Documents\GitHub\Ontology-Overview-of-NFDI4Cat\Master_Table\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Ontology-Overview-of-NFDI4Cat\Master_Table\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A10F53C-457F-4C05-BC45-95D60C8F92F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template mit Beispiel" sheetId="4" r:id="rId1"/>
@@ -31,7 +32,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">BFO!$A$1:$A$93</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1378" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1362" uniqueCount="396">
   <si>
     <t>Ontology</t>
   </si>
@@ -1293,7 +1294,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1792,8 +1793,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2077,14 +2078,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A128"/>
   <sheetViews>
-    <sheetView topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="147.28515625" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
@@ -2587,11 +2588,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A21" r:id="rId1"/>
-    <hyperlink ref="A17" r:id="rId2"/>
-    <hyperlink ref="A19" r:id="rId3"/>
-    <hyperlink ref="A15" r:id="rId4"/>
-    <hyperlink ref="A126" r:id="rId5"/>
+    <hyperlink ref="A21" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A17" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A19" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="A15" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="A126" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200"/>
@@ -2599,14 +2600,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:A95"/>
   <sheetViews>
     <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="147.28515625" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
@@ -3057,11 +3058,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A21" r:id="rId1"/>
-    <hyperlink ref="A17" r:id="rId2"/>
-    <hyperlink ref="A19" r:id="rId3"/>
-    <hyperlink ref="A15" r:id="rId4"/>
-    <hyperlink ref="A23" r:id="rId5"/>
+    <hyperlink ref="A21" r:id="rId1" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink ref="A17" r:id="rId2" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
+    <hyperlink ref="A19" r:id="rId3" xr:uid="{00000000-0004-0000-0900-000002000000}"/>
+    <hyperlink ref="A15" r:id="rId4" xr:uid="{00000000-0004-0000-0900-000003000000}"/>
+    <hyperlink ref="A23" r:id="rId5" xr:uid="{00000000-0004-0000-0900-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200"/>
@@ -3069,14 +3070,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:A93"/>
   <sheetViews>
     <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="148.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="102.5703125" customWidth="1"/>
@@ -3528,14 +3529,14 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:A126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="147.28515625" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
@@ -3998,11 +3999,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A21" r:id="rId1"/>
-    <hyperlink ref="A15" r:id="rId2"/>
-    <hyperlink ref="A23" r:id="rId3"/>
-    <hyperlink ref="A17" r:id="rId4"/>
-    <hyperlink ref="A9" r:id="rId5" display="https://doi.org/10.3030/760907 Virtual Materials Marketplace (VIMMP) project consortium; Andreas Fiseni; Christoph Niethammer; Daniele Toti (ORCID 0000-0002-9668-6961); Gerhard Goldbeck (ORCID 0000-0002-4181-2852); Gianluca Boccardo (ORCID 0000-0003-1264-8237); Helge Krieg; Jadran Vrabec (ORCID 0000-0002-7947-4051); Joshua D. Elliott (ORCID 0000-0002-0729-246X); Mara Chiricotto (ORCID 0000-0003-1609-5254); Paola Carbone (ORCID 0000-0001-9927-8376); Peter Schiffels; Philipp Neumann; Vladimir Lobaskin (ORCID 0000-0002-5231-0639); Welchy Leite Cavalcanti; Ilian T. Todorov (ORCID 0000-0001-7275-1784); Martin Thomas Horsch (ORCID 0000-0002-9464-6739); Michael A. Seaton (ORCID 0000-0002-4708-573X); Silvia Chiacchiera (ORCID 0000-0003-0422-7870)"/>
+    <hyperlink ref="A21" r:id="rId1" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
+    <hyperlink ref="A15" r:id="rId2" xr:uid="{00000000-0004-0000-0B00-000001000000}"/>
+    <hyperlink ref="A23" r:id="rId3" xr:uid="{00000000-0004-0000-0B00-000002000000}"/>
+    <hyperlink ref="A17" r:id="rId4" xr:uid="{00000000-0004-0000-0B00-000003000000}"/>
+    <hyperlink ref="A9" r:id="rId5" display="https://doi.org/10.3030/760907 Virtual Materials Marketplace (VIMMP) project consortium; Andreas Fiseni; Christoph Niethammer; Daniele Toti (ORCID 0000-0002-9668-6961); Gerhard Goldbeck (ORCID 0000-0002-4181-2852); Gianluca Boccardo (ORCID 0000-0003-1264-8237); Helge Krieg; Jadran Vrabec (ORCID 0000-0002-7947-4051); Joshua D. Elliott (ORCID 0000-0002-0729-246X); Mara Chiricotto (ORCID 0000-0003-1609-5254); Paola Carbone (ORCID 0000-0001-9927-8376); Peter Schiffels; Philipp Neumann; Vladimir Lobaskin (ORCID 0000-0002-5231-0639); Welchy Leite Cavalcanti; Ilian T. Todorov (ORCID 0000-0001-7275-1784); Martin Thomas Horsch (ORCID 0000-0002-9464-6739); Michael A. Seaton (ORCID 0000-0002-4708-573X); Silvia Chiacchiera (ORCID 0000-0003-0422-7870)" xr:uid="{00000000-0004-0000-0B00-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200"/>
@@ -4010,14 +4011,14 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:A126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="147.28515625" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
@@ -4483,14 +4484,14 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:F126"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="147.28515625" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
@@ -4954,8 +4955,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A23" r:id="rId1"/>
-    <hyperlink ref="A17" r:id="rId2"/>
+    <hyperlink ref="A23" r:id="rId1" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
+    <hyperlink ref="A17" r:id="rId2" xr:uid="{00000000-0004-0000-0D00-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId3"/>
@@ -4963,14 +4964,14 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:A126"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="147.28515625" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
@@ -5433,12 +5434,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A21" r:id="rId1"/>
-    <hyperlink ref="A15" r:id="rId2"/>
-    <hyperlink ref="A23" r:id="rId3"/>
-    <hyperlink ref="A17" r:id="rId4"/>
-    <hyperlink ref="A9" r:id="rId5" display="https://doi.org/10.3030/760907 Virtual Materials Marketplace (VIMMP) project consortium; Andreas Fiseni; Christoph Niethammer; Daniele Toti (ORCID 0000-0002-9668-6961); Gerhard Goldbeck (ORCID 0000-0002-4181-2852); Gianluca Boccardo (ORCID 0000-0003-1264-8237); Helge Krieg; Jadran Vrabec (ORCID 0000-0002-7947-4051); Joshua D. Elliott (ORCID 0000-0002-0729-246X); Mara Chiricotto (ORCID 0000-0003-1609-5254); Paola Carbone (ORCID 0000-0001-9927-8376); Peter Schiffels; Philipp Neumann; Vladimir Lobaskin (ORCID 0000-0002-5231-0639); Welchy Leite Cavalcanti; Ilian T. Todorov (ORCID 0000-0001-7275-1784); Martin Thomas Horsch (ORCID 0000-0002-9464-6739); Michael A. Seaton (ORCID 0000-0002-4708-573X); Silvia Chiacchiera (ORCID 0000-0003-0422-7870)"/>
-    <hyperlink ref="A19" r:id="rId6"/>
+    <hyperlink ref="A21" r:id="rId1" xr:uid="{00000000-0004-0000-0E00-000000000000}"/>
+    <hyperlink ref="A15" r:id="rId2" xr:uid="{00000000-0004-0000-0E00-000001000000}"/>
+    <hyperlink ref="A23" r:id="rId3" xr:uid="{00000000-0004-0000-0E00-000002000000}"/>
+    <hyperlink ref="A17" r:id="rId4" xr:uid="{00000000-0004-0000-0E00-000003000000}"/>
+    <hyperlink ref="A9" r:id="rId5" display="https://doi.org/10.3030/760907 Virtual Materials Marketplace (VIMMP) project consortium; Andreas Fiseni; Christoph Niethammer; Daniele Toti (ORCID 0000-0002-9668-6961); Gerhard Goldbeck (ORCID 0000-0002-4181-2852); Gianluca Boccardo (ORCID 0000-0003-1264-8237); Helge Krieg; Jadran Vrabec (ORCID 0000-0002-7947-4051); Joshua D. Elliott (ORCID 0000-0002-0729-246X); Mara Chiricotto (ORCID 0000-0003-1609-5254); Paola Carbone (ORCID 0000-0001-9927-8376); Peter Schiffels; Philipp Neumann; Vladimir Lobaskin (ORCID 0000-0002-5231-0639); Welchy Leite Cavalcanti; Ilian T. Todorov (ORCID 0000-0001-7275-1784); Martin Thomas Horsch (ORCID 0000-0002-9464-6739); Michael A. Seaton (ORCID 0000-0002-4708-573X); Silvia Chiacchiera (ORCID 0000-0003-0422-7870)" xr:uid="{00000000-0004-0000-0E00-000004000000}"/>
+    <hyperlink ref="A19" r:id="rId6" xr:uid="{00000000-0004-0000-0E00-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200"/>
@@ -5446,7 +5447,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AU34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5454,7 +5455,7 @@
       <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="71.85546875" defaultRowHeight="69.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="71.85546875" defaultRowHeight="69.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" customWidth="1"/>
@@ -6323,52 +6324,52 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="H2" r:id="rId2"/>
-    <hyperlink ref="G3" r:id="rId3"/>
-    <hyperlink ref="H3" r:id="rId4"/>
-    <hyperlink ref="G4" r:id="rId5"/>
-    <hyperlink ref="H4" r:id="rId6"/>
-    <hyperlink ref="G5" r:id="rId7"/>
-    <hyperlink ref="H5" r:id="rId8"/>
-    <hyperlink ref="G6" r:id="rId9"/>
-    <hyperlink ref="G7" r:id="rId10"/>
-    <hyperlink ref="H7" r:id="rId11"/>
-    <hyperlink ref="G8" r:id="rId12"/>
-    <hyperlink ref="G9" r:id="rId13" location=".YXq72hxCRGo"/>
-    <hyperlink ref="G10" r:id="rId14"/>
-    <hyperlink ref="H10" r:id="rId15"/>
-    <hyperlink ref="G11" r:id="rId16"/>
-    <hyperlink ref="H11" r:id="rId17"/>
-    <hyperlink ref="G12" r:id="rId18"/>
-    <hyperlink ref="H12" r:id="rId19"/>
-    <hyperlink ref="G13" r:id="rId20"/>
-    <hyperlink ref="G14" r:id="rId21"/>
-    <hyperlink ref="G15" r:id="rId22"/>
-    <hyperlink ref="H15" r:id="rId23"/>
-    <hyperlink ref="G17" r:id="rId24" location=".YYVO9LoxlPY"/>
-    <hyperlink ref="H17" r:id="rId25"/>
-    <hyperlink ref="H18" r:id="rId26"/>
-    <hyperlink ref="H19" r:id="rId27"/>
-    <hyperlink ref="G20" r:id="rId28"/>
-    <hyperlink ref="H20" r:id="rId29"/>
-    <hyperlink ref="G21" r:id="rId30"/>
-    <hyperlink ref="G19" r:id="rId31"/>
-    <hyperlink ref="G18" r:id="rId32"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="H2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="G3" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="H3" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="G4" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="H4" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="G5" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="H5" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="G6" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="G7" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="H7" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="G8" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="G9" r:id="rId13" location=".YXq72hxCRGo" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="G10" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="H10" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="G11" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="H11" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="G12" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
+    <hyperlink ref="H12" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
+    <hyperlink ref="G13" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
+    <hyperlink ref="G14" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
+    <hyperlink ref="G15" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
+    <hyperlink ref="H15" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
+    <hyperlink ref="G17" r:id="rId24" location=".YYVO9LoxlPY" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
+    <hyperlink ref="H17" r:id="rId25" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
+    <hyperlink ref="H18" r:id="rId26" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
+    <hyperlink ref="H19" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
+    <hyperlink ref="G20" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
+    <hyperlink ref="H20" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
+    <hyperlink ref="G21" r:id="rId30" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
+    <hyperlink ref="G19" r:id="rId31" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
+    <hyperlink ref="G18" r:id="rId32" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A125"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:A123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81"/>
+    <sheetView topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="A112" sqref="A112"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="147.28515625" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
@@ -6800,107 +6801,41 @@
       <c r="A93" s="36"/>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" s="15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>68</v>
-      </c>
+      <c r="A104" s="15"/>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" s="15" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>71</v>
-      </c>
+      <c r="A110" s="15"/>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" s="15" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>75</v>
-      </c>
+      <c r="A115" s="15"/>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121" s="15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>77</v>
-      </c>
+      <c r="A121" s="15"/>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A123" s="14" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>80</v>
-      </c>
+      <c r="A123" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A21" r:id="rId1"/>
-    <hyperlink ref="A17" r:id="rId2"/>
-    <hyperlink ref="A19" r:id="rId3"/>
-    <hyperlink ref="A15" r:id="rId4"/>
-    <hyperlink ref="A123" r:id="rId5"/>
+    <hyperlink ref="A21" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="A17" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="A19" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="A15" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId6"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A95"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="147.28515625" customWidth="1"/>
   </cols>
@@ -7354,23 +7289,23 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A93"/>
+  <autoFilter ref="A1:A93" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <hyperlinks>
-    <hyperlink ref="A19" r:id="rId1"/>
+    <hyperlink ref="A19" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:A93"/>
   <sheetViews>
     <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="148.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="102.5703125" customWidth="1"/>
@@ -7818,25 +7753,25 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A17" r:id="rId1"/>
-    <hyperlink ref="A21" r:id="rId2"/>
-    <hyperlink ref="A15" r:id="rId3"/>
-    <hyperlink ref="A23" r:id="rId4"/>
-    <hyperlink ref="A39" r:id="rId5"/>
+    <hyperlink ref="A17" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="A21" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="A15" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink ref="A23" r:id="rId4" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
+    <hyperlink ref="A39" r:id="rId5" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:A94"/>
   <sheetViews>
     <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="116.42578125" customWidth="1"/>
   </cols>
@@ -8301,22 +8236,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A9" r:id="rId1" display="doi:10.1007/s13218-020-00648-9; doi:10.1021/acs.jced.9b00739; doi:10.5281/zenodo.3936795; Virtual Materials Marketplace (VIMMP) project consortium;Adham Hashibon; Andrea Scotto di Minico; Andreas Fiseni; Barbara Andreon; Barbora Planková (ORCID 0000-0002-3309-6809); Björn Schembera (ORCID 0000-0003-2860-6621); Christoph Niethammer; Daniele Toti (ORCID 0000-0002-9668-6961); Emanuele Ghedini (ORCID 0000-0003-3805-8761); Esteban Bayro Kaiser (ORCID 0000-0002-5281-0836); Georg J. Schmitz (0000-0003-4065-9742); Gerhard Goldbeck (ORCID 0000-0002-4181-2852); Gianluca Boccardo (ORCID 0000-0003-1264-8237); Hauke Brüning; Helge Krieg; Ignacio Pagonabarraga Mora (ORCID 0000-0002-6187-5025); Jadran Vrabec (ORCID 0000-0002-7947-4051); Javier Díaz Brañas; Jean-Pierre Minier; Joshua D. Elliott (ORCID 0000-0002-0729-246X); Karel Šindelka (ORCID 0000-0003-3925-924X); Mara Chiricotto (ORCID 0000-0003-1609-5254); Martin Lísal (ORCID 0000-0001-8005-7143); Natalia A. Konchakova; Paola Carbone (ORCID 0000-0001-9927-8376); Pascale Noyret; Peter Klein; Peter Schiffels; Philipp Neumann; Vincent Stobiac; Vladimir Lobaskin (ORCID 0000-0002-5231-0639); Welchy Leite Cavalcanti; Youness Bami; Yvan Fournier; Éric Fayolle; Ilian T. Todorov (ORCID 0000-0001-7275-1784); Martin Thomas Horsch (ORCID 0000-0002-9464-6739); Michael A. Seaton (ORCID 0000-0002-4708-573X); Silvia Chiacchiera (ORCID 0000-0003-0422-7870)"/>
-    <hyperlink ref="A23" r:id="rId2"/>
+    <hyperlink ref="A9" r:id="rId1" display="doi:10.1007/s13218-020-00648-9; doi:10.1021/acs.jced.9b00739; doi:10.5281/zenodo.3936795; Virtual Materials Marketplace (VIMMP) project consortium;Adham Hashibon; Andrea Scotto di Minico; Andreas Fiseni; Barbara Andreon; Barbora Planková (ORCID 0000-0002-3309-6809); Björn Schembera (ORCID 0000-0003-2860-6621); Christoph Niethammer; Daniele Toti (ORCID 0000-0002-9668-6961); Emanuele Ghedini (ORCID 0000-0003-3805-8761); Esteban Bayro Kaiser (ORCID 0000-0002-5281-0836); Georg J. Schmitz (0000-0003-4065-9742); Gerhard Goldbeck (ORCID 0000-0002-4181-2852); Gianluca Boccardo (ORCID 0000-0003-1264-8237); Hauke Brüning; Helge Krieg; Ignacio Pagonabarraga Mora (ORCID 0000-0002-6187-5025); Jadran Vrabec (ORCID 0000-0002-7947-4051); Javier Díaz Brañas; Jean-Pierre Minier; Joshua D. Elliott (ORCID 0000-0002-0729-246X); Karel Šindelka (ORCID 0000-0003-3925-924X); Mara Chiricotto (ORCID 0000-0003-1609-5254); Martin Lísal (ORCID 0000-0001-8005-7143); Natalia A. Konchakova; Paola Carbone (ORCID 0000-0001-9927-8376); Pascale Noyret; Peter Klein; Peter Schiffels; Philipp Neumann; Vincent Stobiac; Vladimir Lobaskin (ORCID 0000-0002-5231-0639); Welchy Leite Cavalcanti; Youness Bami; Yvan Fournier; Éric Fayolle; Ilian T. Todorov (ORCID 0000-0001-7275-1784); Martin Thomas Horsch (ORCID 0000-0002-9464-6739); Michael A. Seaton (ORCID 0000-0002-4708-573X); Silvia Chiacchiera (ORCID 0000-0003-0422-7870)" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="A23" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:A126"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="147.28515625" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
@@ -8779,10 +8714,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A21" r:id="rId1"/>
-    <hyperlink ref="A15" r:id="rId2"/>
-    <hyperlink ref="A23" r:id="rId3"/>
-    <hyperlink ref="A17" r:id="rId4"/>
+    <hyperlink ref="A21" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="A15" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
+    <hyperlink ref="A23" r:id="rId3" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
+    <hyperlink ref="A17" r:id="rId4" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200"/>
@@ -8790,14 +8725,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:A95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="147.28515625" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
@@ -9241,9 +9176,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A21" r:id="rId1"/>
-    <hyperlink ref="A17" r:id="rId2"/>
-    <hyperlink ref="A15" r:id="rId3"/>
+    <hyperlink ref="A21" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
+    <hyperlink ref="A17" r:id="rId2" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
+    <hyperlink ref="A15" r:id="rId3" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200"/>
@@ -9251,14 +9186,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:A95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="147.28515625" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
@@ -9709,7 +9644,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A17" r:id="rId1"/>
+    <hyperlink ref="A17" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId2"/>
@@ -9726,6 +9661,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="文档" ma:contentTypeID="0x010100E35C4A3F015220429587A6885988F55A" ma:contentTypeVersion="2" ma:contentTypeDescription="新建文档。" ma:contentTypeScope="" ma:versionID="d6504310574d90ff3af330d88d4b27c4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="43c33c4e-3078-430a-a993-ec9e07a267b1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7023e3b9e2c813b12cebe0f0ea1d5cce" ns2:_="">
     <xsd:import namespace="43c33c4e-3078-430a-a993-ec9e07a267b1"/>
@@ -9857,12 +9798,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4E38D5B-D85B-4D43-8837-BDE8BD7F5B8A}">
   <ds:schemaRefs>
@@ -9872,6 +9807,15 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0CE3216-5465-401D-96FE-F0724F372422}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3709C412-EE61-448D-9135-2444D463CA94}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9887,13 +9831,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0CE3216-5465-401D-96FE-F0724F372422}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>